<commit_message>
Buscador. Fix del provider.json. Instalacion de herramientas
</commit_message>
<xml_diff>
--- a/MigrationScripts/Data/Proveedores.xlsx
+++ b/MigrationScripts/Data/Proveedores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">numeroCuenta</t>
   </si>
   <si>
-    <t xml:space="preserve">nombreContacto </t>
+    <t xml:space="preserve">nombreContacto</t>
   </si>
   <si>
     <t xml:space="preserve">apellidoContacto</t>
@@ -262,6 +262,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -353,18 +354,18 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +709,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>